<commit_message>
#Update Trends and slight adjustments
</commit_message>
<xml_diff>
--- a/data/Economic_Impact/GDP/C_Percentage change in regional GDP.xlsx
+++ b/data/Economic_Impact/GDP/C_Percentage change in regional GDP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Konstantin\Desktop\Dashboard_Vers1\data\Economic_Impact\GDP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81831D36-39E2-4FD0-AA56-20737128C651}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E6D054-C082-4CBB-847E-31FED031BA6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19665" yWindow="3180" windowWidth="29985" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="29985" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 2.8" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>OECD Europe</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>Latin America</t>
-  </si>
-  <si>
-    <t>World</t>
   </si>
   <si>
     <t>South and South-East Asia</t>
@@ -541,27 +538,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J869"/>
+  <dimension ref="A1:I869"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="AA6" sqref="AA6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="3" width="9.7109375" customWidth="1"/>
-    <col min="4" max="5" width="8.42578125" customWidth="1"/>
-    <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="8" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="8" customWidth="1"/>
-    <col min="10" max="10" width="8.42578125" customWidth="1"/>
-    <col min="11" max="26" width="8" customWidth="1"/>
+    <col min="4" max="7" width="8.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" customWidth="1"/>
+    <col min="10" max="25" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -576,22 +571,19 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>2010</v>
       </c>
@@ -602,10 +594,9 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>2011</v>
       </c>
@@ -622,22 +613,19 @@
         <v>-1.1764054718753636E-3</v>
       </c>
       <c r="F3" s="8">
-        <v>-6.2534917500600695E-4</v>
+        <v>-1.2448275338414749E-3</v>
       </c>
       <c r="G3" s="8">
-        <v>-1.2448275338414749E-3</v>
+        <v>-1.2942818439776183E-3</v>
       </c>
       <c r="H3" s="8">
-        <v>-1.2942818439776183E-3</v>
-      </c>
-      <c r="I3" s="8">
         <v>-1.4798890658047625E-3</v>
       </c>
-      <c r="J3" s="9">
+      <c r="I3" s="9">
         <v>-1.9161103098351839E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10">
         <v>2012</v>
       </c>
@@ -654,22 +642,19 @@
         <v>-1.3356193794052951E-3</v>
       </c>
       <c r="F4" s="11">
-        <v>-7.5642133725395411E-4</v>
+        <v>-1.5583200837027134E-3</v>
       </c>
       <c r="G4" s="11">
-        <v>-1.5583200837027134E-3</v>
+        <v>-1.5305345949639948E-3</v>
       </c>
       <c r="H4" s="11">
-        <v>-1.5305345949639948E-3</v>
-      </c>
-      <c r="I4" s="11">
         <v>-1.6890137609872902E-3</v>
       </c>
-      <c r="J4" s="12">
+      <c r="I4" s="12">
         <v>-2.0798676199915711E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>2013</v>
       </c>
@@ -686,22 +671,19 @@
         <v>-1.5644170949855596E-3</v>
       </c>
       <c r="F5" s="8">
-        <v>-9.1782746021129569E-4</v>
+        <v>-1.8044249090919395E-3</v>
       </c>
       <c r="G5" s="8">
-        <v>-1.8044249090919395E-3</v>
+        <v>-1.8486831664825676E-3</v>
       </c>
       <c r="H5" s="8">
-        <v>-1.8486831664825676E-3</v>
-      </c>
-      <c r="I5" s="8">
         <v>-2.0222670361813577E-3</v>
       </c>
-      <c r="J5" s="9">
+      <c r="I5" s="9">
         <v>-2.4886241583650381E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="10">
         <v>2014</v>
       </c>
@@ -718,22 +700,19 @@
         <v>-1.7771016306462606E-3</v>
       </c>
       <c r="F6" s="11">
-        <v>-1.0810518671192648E-3</v>
+        <v>-2.0613402139242343E-3</v>
       </c>
       <c r="G6" s="11">
-        <v>-2.0613402139242343E-3</v>
+        <v>-2.1055371318203786E-3</v>
       </c>
       <c r="H6" s="11">
-        <v>-2.1055371318203786E-3</v>
-      </c>
-      <c r="I6" s="11">
         <v>-2.3722922723254936E-3</v>
       </c>
-      <c r="J6" s="12">
+      <c r="I6" s="12">
         <v>-2.8861171233375282E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>2015</v>
       </c>
@@ -750,22 +729,19 @@
         <v>-1.990253718880175E-3</v>
       </c>
       <c r="F7" s="8">
-        <v>-1.2462548047735833E-3</v>
+        <v>-2.3150333105144139E-3</v>
       </c>
       <c r="G7" s="8">
-        <v>-2.3150333105144139E-3</v>
+        <v>-2.428283346418425E-3</v>
       </c>
       <c r="H7" s="8">
-        <v>-2.428283346418425E-3</v>
-      </c>
-      <c r="I7" s="8">
         <v>-2.7372571082631136E-3</v>
       </c>
-      <c r="J7" s="9">
+      <c r="I7" s="9">
         <v>-3.2789644393675932E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10">
         <v>2016</v>
       </c>
@@ -782,22 +758,19 @@
         <v>-2.2195165699904207E-3</v>
       </c>
       <c r="F8" s="11">
-        <v>-1.4329940907436001E-3</v>
+        <v>-2.6200983761990315E-3</v>
       </c>
       <c r="G8" s="11">
-        <v>-2.6200983761990315E-3</v>
+        <v>-2.801838239119725E-3</v>
       </c>
       <c r="H8" s="11">
-        <v>-2.801838239119725E-3</v>
-      </c>
-      <c r="I8" s="11">
         <v>-3.1293780530130544E-3</v>
       </c>
-      <c r="J8" s="12">
+      <c r="I8" s="12">
         <v>-3.6769412462578366E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>2017</v>
       </c>
@@ -814,22 +787,19 @@
         <v>-2.4541859615587747E-3</v>
       </c>
       <c r="F9" s="8">
-        <v>-1.6259258292277146E-3</v>
+        <v>-2.9151718446467356E-3</v>
       </c>
       <c r="G9" s="8">
-        <v>-2.9151718446467356E-3</v>
+        <v>-3.1960620854318833E-3</v>
       </c>
       <c r="H9" s="8">
-        <v>-3.1960620854318833E-3</v>
-      </c>
-      <c r="I9" s="8">
         <v>-3.5292329064472439E-3</v>
       </c>
-      <c r="J9" s="9">
+      <c r="I9" s="9">
         <v>-4.0812567655899024E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10">
         <v>2018</v>
       </c>
@@ -846,22 +816,19 @@
         <v>-2.6898875228809072E-3</v>
       </c>
       <c r="F10" s="11">
-        <v>-1.8239396994101931E-3</v>
+        <v>-3.202369787149828E-3</v>
       </c>
       <c r="G10" s="11">
-        <v>-3.202369787149828E-3</v>
+        <v>-3.6027529693081206E-3</v>
       </c>
       <c r="H10" s="11">
-        <v>-3.6027529693081206E-3</v>
-      </c>
-      <c r="I10" s="11">
         <v>-3.93435900973782E-3</v>
       </c>
-      <c r="J10" s="12">
+      <c r="I10" s="12">
         <v>-4.4957880204685718E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>2019</v>
       </c>
@@ -878,22 +845,19 @@
         <v>-2.9244640077056294E-3</v>
       </c>
       <c r="F11" s="8">
-        <v>-2.0246373794844397E-3</v>
+        <v>-3.4915346698198846E-3</v>
       </c>
       <c r="G11" s="8">
-        <v>-3.4915346698198846E-3</v>
+        <v>-4.0145258850771137E-3</v>
       </c>
       <c r="H11" s="8">
-        <v>-4.0145258850771137E-3</v>
-      </c>
-      <c r="I11" s="8">
         <v>-4.3391481664690756E-3</v>
       </c>
-      <c r="J11" s="9">
+      <c r="I11" s="9">
         <v>-4.8662865760837892E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="10">
         <v>2020</v>
       </c>
@@ -910,22 +874,19 @@
         <v>-3.1682880001981939E-3</v>
       </c>
       <c r="F12" s="11">
-        <v>-2.2350924992315946E-3</v>
+        <v>-3.7848561082123311E-3</v>
       </c>
       <c r="G12" s="11">
-        <v>-3.7848561082123311E-3</v>
+        <v>-4.4495117532369344E-3</v>
       </c>
       <c r="H12" s="11">
-        <v>-4.4495117532369344E-3</v>
-      </c>
-      <c r="I12" s="11">
         <v>-4.7513834574614E-3</v>
       </c>
-      <c r="J12" s="12">
+      <c r="I12" s="12">
         <v>-5.2761852898530748E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7">
         <v>2021</v>
       </c>
@@ -942,22 +903,19 @@
         <v>-3.4249237820543899E-3</v>
       </c>
       <c r="F13" s="8">
-        <v>-2.4274341781227449E-3</v>
+        <v>-4.0592026228861711E-3</v>
       </c>
       <c r="G13" s="8">
-        <v>-4.0592026228861711E-3</v>
+        <v>-4.889402844606483E-3</v>
       </c>
       <c r="H13" s="8">
-        <v>-4.889402844606483E-3</v>
-      </c>
-      <c r="I13" s="8">
         <v>-5.1498811187447036E-3</v>
       </c>
-      <c r="J13" s="9">
+      <c r="I13" s="9">
         <v>-5.6731380855488123E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10">
         <v>2022</v>
       </c>
@@ -974,22 +932,19 @@
         <v>-3.6829429360413224E-3</v>
       </c>
       <c r="F14" s="11">
-        <v>-2.631347798400907E-3</v>
+        <v>-4.3379034632935465E-3</v>
       </c>
       <c r="G14" s="11">
-        <v>-4.3379034632935465E-3</v>
+        <v>-5.34901312337277E-3</v>
       </c>
       <c r="H14" s="11">
-        <v>-5.34901312337277E-3</v>
-      </c>
-      <c r="I14" s="11">
         <v>-5.5672747650244991E-3</v>
       </c>
-      <c r="J14" s="12">
+      <c r="I14" s="12">
         <v>-6.0790285834960711E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7">
         <v>2023</v>
       </c>
@@ -1006,22 +961,19 @@
         <v>-3.9336004559210602E-3</v>
       </c>
       <c r="F15" s="8">
-        <v>-2.8452361048878494E-3</v>
+        <v>-4.6229568974752722E-3</v>
       </c>
       <c r="G15" s="8">
-        <v>-4.6229568974752722E-3</v>
+        <v>-5.818732324056608E-3</v>
       </c>
       <c r="H15" s="8">
-        <v>-5.818732324056608E-3</v>
-      </c>
-      <c r="I15" s="8">
         <v>-6.0015006492237788E-3</v>
       </c>
-      <c r="J15" s="9">
+      <c r="I15" s="9">
         <v>-6.4958529626768513E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="10">
         <v>2024</v>
       </c>
@@ -1038,22 +990,19 @@
         <v>-4.1857691462543478E-3</v>
       </c>
       <c r="F16" s="11">
-        <v>-3.0695904695580145E-3</v>
+        <v>-4.9130995915811493E-3</v>
       </c>
       <c r="G16" s="11">
-        <v>-4.9130995915811493E-3</v>
+        <v>-6.3003041263843818E-3</v>
       </c>
       <c r="H16" s="11">
-        <v>-6.3003041263843818E-3</v>
-      </c>
-      <c r="I16" s="11">
         <v>-6.4516948422840281E-3</v>
       </c>
-      <c r="J16" s="12">
+      <c r="I16" s="12">
         <v>-6.9243760785148156E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7">
         <v>2025</v>
       </c>
@@ -1070,22 +1019,19 @@
         <v>-4.4385136125457691E-3</v>
       </c>
       <c r="F17" s="8">
-        <v>-3.3032840368661942E-3</v>
+        <v>-5.2081208272849455E-3</v>
       </c>
       <c r="G17" s="8">
-        <v>-5.2081208272849455E-3</v>
+        <v>-6.7963761032208136E-3</v>
       </c>
       <c r="H17" s="8">
-        <v>-6.7963761032208136E-3</v>
-      </c>
-      <c r="I17" s="8">
         <v>-6.9159344929922151E-3</v>
       </c>
-      <c r="J17" s="9">
+      <c r="I17" s="9">
         <v>-7.3650461567260628E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10">
         <v>2026</v>
       </c>
@@ -1102,22 +1048,19 @@
         <v>-4.7143733482164496E-3</v>
       </c>
       <c r="F18" s="11">
-        <v>-3.5650650966148056E-3</v>
+        <v>-5.5493848384756683E-3</v>
       </c>
       <c r="G18" s="11">
-        <v>-5.5493848384756683E-3</v>
+        <v>-7.3512457645362739E-3</v>
       </c>
       <c r="H18" s="11">
-        <v>-7.3512457645362739E-3</v>
-      </c>
-      <c r="I18" s="11">
         <v>-7.4239304040497611E-3</v>
       </c>
-      <c r="J18" s="12">
+      <c r="I18" s="12">
         <v>-7.8520807318702701E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7">
         <v>2027</v>
       </c>
@@ -1134,22 +1077,19 @@
         <v>-4.9893861913544724E-3</v>
       </c>
       <c r="F19" s="8">
-        <v>-3.8333933373139173E-3</v>
+        <v>-5.885577189948088E-3</v>
       </c>
       <c r="G19" s="8">
-        <v>-5.885577189948088E-3</v>
+        <v>-7.9236351724578657E-3</v>
       </c>
       <c r="H19" s="8">
-        <v>-7.9236351724578657E-3</v>
-      </c>
-      <c r="I19" s="8">
         <v>-7.9412792402735466E-3</v>
       </c>
-      <c r="J19" s="9">
+      <c r="I19" s="9">
         <v>-8.3518751096260946E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10">
         <v>2028</v>
       </c>
@@ -1166,22 +1106,19 @@
         <v>-5.2643812377305421E-3</v>
       </c>
       <c r="F20" s="11">
-        <v>-4.1085753817254878E-3</v>
+        <v>-6.2202540729570099E-3</v>
       </c>
       <c r="G20" s="11">
-        <v>-6.2202540729570099E-3</v>
+        <v>-8.5048188873646513E-3</v>
       </c>
       <c r="H20" s="11">
-        <v>-8.5048188873646513E-3</v>
-      </c>
-      <c r="I20" s="11">
         <v>-8.4685794268412051E-3</v>
       </c>
-      <c r="J20" s="12">
+      <c r="I20" s="12">
         <v>-8.8601394467746619E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7">
         <v>2029</v>
       </c>
@@ -1198,22 +1135,19 @@
         <v>-5.5396782364321995E-3</v>
       </c>
       <c r="F21" s="8">
-        <v>-4.3922997530951857E-3</v>
+        <v>-6.5558976155460913E-3</v>
       </c>
       <c r="G21" s="8">
-        <v>-6.5558976155460913E-3</v>
+        <v>-9.103922452440294E-3</v>
       </c>
       <c r="H21" s="8">
-        <v>-9.103922452440294E-3</v>
-      </c>
-      <c r="I21" s="8">
         <v>-9.0070103838948423E-3</v>
       </c>
-      <c r="J21" s="9">
+      <c r="I21" s="9">
         <v>-9.3833696536680389E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="10">
         <v>2030</v>
       </c>
@@ -1230,22 +1164,19 @@
         <v>-5.8170197351390396E-3</v>
       </c>
       <c r="F22" s="11">
-        <v>-4.6856422519970797E-3</v>
+        <v>-6.8963420688191723E-3</v>
       </c>
       <c r="G22" s="11">
-        <v>-6.8963420688191723E-3</v>
+        <v>-9.7136576747008929E-3</v>
       </c>
       <c r="H22" s="11">
-        <v>-9.7136576747008929E-3</v>
-      </c>
-      <c r="I22" s="11">
         <v>-9.5583915675790943E-3</v>
       </c>
-      <c r="J22" s="12">
+      <c r="I22" s="12">
         <v>-9.9232945495256741E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7">
         <v>2031</v>
       </c>
@@ -1262,22 +1193,19 @@
         <v>-6.1126499500150366E-3</v>
       </c>
       <c r="F23" s="8">
-        <v>-5.0022999333082518E-3</v>
+        <v>-7.2708897714194309E-3</v>
       </c>
       <c r="G23" s="8">
-        <v>-7.2708897714194309E-3</v>
+        <v>-1.0369993268981137E-2</v>
       </c>
       <c r="H23" s="8">
-        <v>-1.0369993268981137E-2</v>
-      </c>
-      <c r="I23" s="8">
         <v>-1.0144786296308883E-2</v>
       </c>
-      <c r="J23" s="9">
+      <c r="I23" s="9">
         <v>-1.0507797905065286E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10">
         <v>2032</v>
       </c>
@@ -1294,22 +1222,19 @@
         <v>-6.40744414362171E-3</v>
       </c>
       <c r="F24" s="11">
-        <v>-5.3288066145436019E-3</v>
+        <v>-7.6450325832907451E-3</v>
       </c>
       <c r="G24" s="11">
-        <v>-7.6450325832907451E-3</v>
+        <v>-1.1043929981288336E-2</v>
       </c>
       <c r="H24" s="11">
-        <v>-1.1043929981288336E-2</v>
-      </c>
-      <c r="I24" s="11">
         <v>-1.0747559314391086E-2</v>
       </c>
-      <c r="J24" s="12">
+      <c r="I24" s="12">
         <v>-1.1109571536647045E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7">
         <v>2033</v>
       </c>
@@ -1326,22 +1251,19 @@
         <v>-6.7030211507224102E-3</v>
       </c>
       <c r="F25" s="8">
-        <v>-5.666144412971974E-3</v>
+        <v>-8.0230292078541376E-3</v>
       </c>
       <c r="G25" s="8">
-        <v>-8.0230292078541376E-3</v>
+        <v>-1.1734183386001518E-2</v>
       </c>
       <c r="H25" s="8">
-        <v>-1.1734183386001518E-2</v>
-      </c>
-      <c r="I25" s="8">
         <v>-1.1363832723633505E-2</v>
       </c>
-      <c r="J25" s="9">
+      <c r="I25" s="9">
         <v>-1.1730838979163605E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="10">
         <v>2034</v>
       </c>
@@ -1358,22 +1280,19 @@
         <v>-7.0003342210804842E-3</v>
       </c>
       <c r="F26" s="11">
-        <v>-6.0158324186173617E-3</v>
+        <v>-8.4072756868945886E-3</v>
       </c>
       <c r="G26" s="11">
-        <v>-8.4072756868945886E-3</v>
+        <v>-1.2444309089019834E-2</v>
       </c>
       <c r="H26" s="11">
-        <v>-1.2444309089019834E-2</v>
-      </c>
-      <c r="I26" s="11">
         <v>-1.1997756717216035E-2</v>
       </c>
-      <c r="J26" s="12">
+      <c r="I26" s="12">
         <v>-1.2372931048820091E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7">
         <v>2035</v>
       </c>
@@ -1390,22 +1309,19 @@
         <v>-7.2993477069018819E-3</v>
       </c>
       <c r="F27" s="8">
-        <v>-6.3777719451971748E-3</v>
+        <v>-8.799402724715133E-3</v>
       </c>
       <c r="G27" s="8">
-        <v>-8.799402724715133E-3</v>
+        <v>-1.3169952530215356E-2</v>
       </c>
       <c r="H27" s="8">
-        <v>-1.3169952530215356E-2</v>
-      </c>
-      <c r="I27" s="8">
         <v>-1.26480666389861E-2</v>
       </c>
-      <c r="J27" s="9">
+      <c r="I27" s="9">
         <v>-1.3038061771063036E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
         <v>2036</v>
       </c>
@@ -1422,22 +1338,19 @@
         <v>-7.6074527159347705E-3</v>
       </c>
       <c r="F28" s="11">
-        <v>-6.7650934758098913E-3</v>
+        <v>-9.239891802885758E-3</v>
       </c>
       <c r="G28" s="11">
-        <v>-9.239891802885758E-3</v>
+        <v>-1.3992365311204513E-2</v>
       </c>
       <c r="H28" s="11">
-        <v>-1.3992365311204513E-2</v>
-      </c>
-      <c r="I28" s="11">
         <v>-1.3277226640937556E-2</v>
       </c>
-      <c r="J28" s="12">
+      <c r="I28" s="12">
         <v>-1.3781453576870106E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7">
         <v>2037</v>
       </c>
@@ -1454,22 +1367,19 @@
         <v>-7.9166204392714379E-3</v>
       </c>
       <c r="F29" s="8">
-        <v>-7.1614412902204494E-3</v>
+        <v>-9.6814056087198841E-3</v>
       </c>
       <c r="G29" s="8">
-        <v>-9.6814056087198841E-3</v>
+        <v>-1.4814180003577815E-2</v>
       </c>
       <c r="H29" s="8">
-        <v>-1.4814180003577815E-2</v>
-      </c>
-      <c r="I29" s="8">
         <v>-1.3921109979173618E-2</v>
       </c>
-      <c r="J29" s="9">
+      <c r="I29" s="9">
         <v>-1.4543029320063572E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="10">
         <v>2038</v>
       </c>
@@ -1486,22 +1396,19 @@
         <v>-8.226842139519297E-3</v>
       </c>
       <c r="F30" s="11">
-        <v>-7.5681874311657182E-3</v>
+        <v>-1.0125338059515987E-2</v>
       </c>
       <c r="G30" s="11">
-        <v>-1.0125338059515987E-2</v>
+        <v>-1.5636690098265849E-2</v>
       </c>
       <c r="H30" s="11">
-        <v>-1.5636690098265849E-2</v>
-      </c>
-      <c r="I30" s="11">
         <v>-1.4585132456043759E-2</v>
       </c>
-      <c r="J30" s="12">
+      <c r="I30" s="12">
         <v>-1.5325375589158585E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7">
         <v>2039</v>
       </c>
@@ -1518,22 +1425,19 @@
         <v>-8.5383331537824958E-3</v>
       </c>
       <c r="F31" s="8">
-        <v>-7.9862213248798053E-3</v>
+        <v>-1.0576077652455718E-2</v>
       </c>
       <c r="G31" s="8">
-        <v>-1.0576077652455718E-2</v>
+        <v>-1.6464211105479576E-2</v>
       </c>
       <c r="H31" s="8">
-        <v>-1.6464211105479576E-2</v>
-      </c>
-      <c r="I31" s="8">
         <v>-1.5264977235790123E-2</v>
       </c>
-      <c r="J31" s="9">
+      <c r="I31" s="9">
         <v>-1.6131543719691832E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="10">
         <v>2040</v>
       </c>
@@ -1550,22 +1454,19 @@
         <v>-8.8492644644223573E-3</v>
       </c>
       <c r="F32" s="11">
-        <v>-8.4156368761709732E-3</v>
+        <v>-1.1034574243755646E-2</v>
       </c>
       <c r="G32" s="11">
-        <v>-1.1034574243755646E-2</v>
+        <v>-1.7297152660832427E-2</v>
       </c>
       <c r="H32" s="11">
-        <v>-1.7297152660832427E-2</v>
-      </c>
-      <c r="I32" s="11">
         <v>-1.5960000097757554E-2</v>
       </c>
-      <c r="J32" s="12">
+      <c r="I32" s="12">
         <v>-1.6963609494705656E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7">
         <v>2041</v>
       </c>
@@ -1582,22 +1483,19 @@
         <v>-9.1540993857863739E-3</v>
       </c>
       <c r="F33" s="8">
-        <v>-8.8649726042195898E-3</v>
+        <v>-1.1513203524088911E-2</v>
       </c>
       <c r="G33" s="8">
-        <v>-1.1513203524088911E-2</v>
+        <v>-1.8157861383538809E-2</v>
       </c>
       <c r="H33" s="8">
-        <v>-1.8157861383538809E-2</v>
-      </c>
-      <c r="I33" s="8">
         <v>-1.671158996953559E-2</v>
       </c>
-      <c r="J33" s="9">
+      <c r="I33" s="9">
         <v>-1.7857514425608456E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="10">
         <v>2042</v>
       </c>
@@ -1614,22 +1512,19 @@
         <v>-9.4565988799497624E-3</v>
       </c>
       <c r="F34" s="11">
-        <v>-9.323437334481377E-3</v>
+        <v>-1.199711574588247E-2</v>
       </c>
       <c r="G34" s="11">
-        <v>-1.199711574588247E-2</v>
+        <v>-1.9003617367794878E-2</v>
       </c>
       <c r="H34" s="11">
-        <v>-1.9003617367794878E-2</v>
-      </c>
-      <c r="I34" s="11">
         <v>-1.7474974966618873E-2</v>
       </c>
-      <c r="J34" s="12">
+      <c r="I34" s="12">
         <v>-1.8776870057668149E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7">
         <v>2043</v>
       </c>
@@ -1646,22 +1541,19 @@
         <v>-9.7620238066438159E-3</v>
       </c>
       <c r="F35" s="8">
-        <v>-9.7924317400904792E-3</v>
+        <v>-1.2489397180307726E-2</v>
       </c>
       <c r="G35" s="8">
-        <v>-1.2489397180307726E-2</v>
+        <v>-1.9836837429034859E-2</v>
       </c>
       <c r="H35" s="8">
-        <v>-1.9836837429034859E-2</v>
-      </c>
-      <c r="I35" s="8">
         <v>-1.8254248744921431E-2</v>
       </c>
-      <c r="J35" s="9">
+      <c r="I35" s="9">
         <v>-1.9713729291181759E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="10">
         <v>2044</v>
       </c>
@@ -1678,22 +1570,19 @@
         <v>-1.0071232108878725E-2</v>
       </c>
       <c r="F36" s="11">
-        <v>-1.0273488519980667E-2</v>
+        <v>-1.2989391019722851E-2</v>
       </c>
       <c r="G36" s="11">
-        <v>-1.2989391019722851E-2</v>
+        <v>-2.0658435061079228E-2</v>
       </c>
       <c r="H36" s="11">
-        <v>-2.0658435061079228E-2</v>
-      </c>
-      <c r="I36" s="11">
         <v>-1.9053462241137353E-2</v>
       </c>
-      <c r="J36" s="12">
+      <c r="I36" s="12">
         <v>-2.0694043588257216E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="7">
         <v>2045</v>
       </c>
@@ -1710,22 +1599,19 @@
         <v>-1.0390439484747382E-2</v>
       </c>
       <c r="F37" s="8">
-        <v>-1.0765982168635557E-2</v>
+        <v>-1.3498297810889293E-2</v>
       </c>
       <c r="G37" s="8">
-        <v>-1.3498297810889293E-2</v>
+        <v>-2.1478337107656231E-2</v>
       </c>
       <c r="H37" s="8">
-        <v>-2.1478337107656231E-2</v>
-      </c>
-      <c r="I37" s="8">
         <v>-1.9877396550061155E-2</v>
       </c>
-      <c r="J37" s="9">
+      <c r="I37" s="9">
         <v>-2.1639497485274273E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="10">
         <v>2046</v>
       </c>
@@ -1742,22 +1628,19 @@
         <v>-1.0718894464247564E-2</v>
       </c>
       <c r="F38" s="11">
-        <v>-1.1287275742131175E-2</v>
+        <v>-1.4034482920797453E-2</v>
       </c>
       <c r="G38" s="11">
-        <v>-1.4034482920797453E-2</v>
+        <v>-2.230791016203082E-2</v>
       </c>
       <c r="H38" s="11">
-        <v>-2.230791016203082E-2</v>
-      </c>
-      <c r="I38" s="11">
         <v>-2.0738994664187937E-2</v>
       </c>
-      <c r="J38" s="12">
+      <c r="I38" s="12">
         <v>-2.2878236542920427E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7">
         <v>2047</v>
       </c>
@@ -1774,22 +1657,19 @@
         <v>-1.1071475555686661E-2</v>
       </c>
       <c r="F39" s="8">
-        <v>-1.1808339379975497E-2</v>
+        <v>-1.458157850500863E-2</v>
       </c>
       <c r="G39" s="8">
-        <v>-1.458157850500863E-2</v>
+        <v>-2.3169834856403559E-2</v>
       </c>
       <c r="H39" s="8">
-        <v>-2.3169834856403559E-2</v>
-      </c>
-      <c r="I39" s="8">
         <v>-2.1640191954300003E-2</v>
       </c>
-      <c r="J39" s="9">
+      <c r="I39" s="9">
         <v>-2.4028443033877567E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10">
         <v>2048</v>
       </c>
@@ -1806,22 +1686,19 @@
         <v>-1.1357519412222405E-2</v>
       </c>
       <c r="F40" s="11">
-        <v>-1.2375837397213374E-2</v>
+        <v>-1.50972942525891E-2</v>
       </c>
       <c r="G40" s="11">
-        <v>-1.50972942525891E-2</v>
+        <v>-2.3866083789764403E-2</v>
       </c>
       <c r="H40" s="11">
-        <v>-2.3866083789764403E-2</v>
-      </c>
-      <c r="I40" s="11">
         <v>-2.2513521706407302E-2</v>
       </c>
-      <c r="J40" s="12">
+      <c r="I40" s="12">
         <v>-2.5007893420120532E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7">
         <v>2049</v>
       </c>
@@ -1838,22 +1715,19 @@
         <v>-1.1759502779568942E-2</v>
       </c>
       <c r="F41" s="8">
-        <v>-1.2928168606730295E-2</v>
+        <v>-1.565959186713628E-2</v>
       </c>
       <c r="G41" s="8">
-        <v>-1.565959186713628E-2</v>
+        <v>-2.4738629022955982E-2</v>
       </c>
       <c r="H41" s="8">
-        <v>-2.4738629022955982E-2</v>
-      </c>
-      <c r="I41" s="8">
         <v>-2.3478152387248818E-2</v>
       </c>
-      <c r="J41" s="9">
+      <c r="I41" s="9">
         <v>-2.6112758365206858E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="10">
         <v>2050</v>
       </c>
@@ -1870,22 +1744,19 @@
         <v>-1.2138652868625588E-2</v>
       </c>
       <c r="F42" s="11">
-        <v>-1.3477948791287608E-2</v>
+        <v>-1.6242004197814297E-2</v>
       </c>
       <c r="G42" s="11">
-        <v>-1.6242004197814297E-2</v>
+        <v>-2.5619998743693251E-2</v>
       </c>
       <c r="H42" s="11">
-        <v>-2.5619998743693251E-2</v>
-      </c>
-      <c r="I42" s="11">
         <v>-2.4495040882939523E-2</v>
       </c>
-      <c r="J42" s="12">
+      <c r="I42" s="12">
         <v>-2.7359486035868553E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7">
         <v>2051</v>
       </c>
@@ -1902,22 +1773,19 @@
         <v>-1.2422380536735611E-2</v>
       </c>
       <c r="F43" s="8">
-        <v>-1.4087189287714241E-2</v>
+        <v>-1.6752441218538139E-2</v>
       </c>
       <c r="G43" s="8">
-        <v>-1.6752441218538139E-2</v>
+        <v>-2.6406394475234074E-2</v>
       </c>
       <c r="H43" s="8">
-        <v>-2.6406394475234074E-2</v>
-      </c>
-      <c r="I43" s="8">
         <v>-2.5551719722424093E-2</v>
       </c>
-      <c r="J43" s="9">
+      <c r="I43" s="9">
         <v>-2.8279931588512341E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="10">
         <v>2052</v>
       </c>
@@ -1934,22 +1802,19 @@
         <v>-1.2758432986215706E-2</v>
       </c>
       <c r="F44" s="11">
-        <v>-1.467801352686926E-2</v>
+        <v>-1.7242285276200753E-2</v>
       </c>
       <c r="G44" s="11">
-        <v>-1.7242285276200753E-2</v>
+        <v>-2.7167032712479777E-2</v>
       </c>
       <c r="H44" s="11">
-        <v>-2.7167032712479777E-2</v>
-      </c>
-      <c r="I44" s="11">
         <v>-2.6616732742074878E-2</v>
       </c>
-      <c r="J44" s="12">
+      <c r="I44" s="12">
         <v>-2.9268304729995354E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="7">
         <v>2053</v>
       </c>
@@ -1966,22 +1831,19 @@
         <v>-1.3110375137657559E-2</v>
       </c>
       <c r="F45" s="8">
-        <v>-1.5273261656158832E-2</v>
+        <v>-1.775034147736454E-2</v>
       </c>
       <c r="G45" s="8">
-        <v>-1.775034147736454E-2</v>
+        <v>-2.7973888280229176E-2</v>
       </c>
       <c r="H45" s="8">
-        <v>-2.7973888280229176E-2</v>
-      </c>
-      <c r="I45" s="8">
         <v>-2.7743114980419592E-2</v>
       </c>
-      <c r="J45" s="9">
+      <c r="I45" s="9">
         <v>-3.049653666883918E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="10">
         <v>2054</v>
       </c>
@@ -1998,22 +1860,19 @@
         <v>-1.3446107980310984E-2</v>
       </c>
       <c r="F46" s="11">
-        <v>-1.5886329676628286E-2</v>
+        <v>-1.8233223901249151E-2</v>
       </c>
       <c r="G46" s="11">
-        <v>-1.8233223901249151E-2</v>
+        <v>-2.8753320336812549E-2</v>
       </c>
       <c r="H46" s="11">
-        <v>-2.8753320336812549E-2</v>
-      </c>
-      <c r="I46" s="11">
         <v>-2.8903079031319834E-2</v>
       </c>
-      <c r="J46" s="12">
+      <c r="I46" s="12">
         <v>-3.1601342781677165E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="7">
         <v>2055</v>
       </c>
@@ -2030,22 +1889,19 @@
         <v>-1.376179237679398E-2</v>
       </c>
       <c r="F47" s="8">
-        <v>-1.6528273662823612E-2</v>
+        <v>-1.8721351435920242E-2</v>
       </c>
       <c r="G47" s="8">
-        <v>-1.8721351435920242E-2</v>
+        <v>-2.9508799160569699E-2</v>
       </c>
       <c r="H47" s="8">
-        <v>-2.9508799160569699E-2</v>
-      </c>
-      <c r="I47" s="8">
         <v>-3.0105044923110169E-2</v>
       </c>
-      <c r="J47" s="9">
+      <c r="I47" s="9">
         <v>-3.2677909110708225E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="10">
         <v>2056</v>
       </c>
@@ -2062,22 +1918,19 @@
         <v>-1.4088582434447883E-2</v>
       </c>
       <c r="F48" s="11">
-        <v>-1.7185191523900967E-2</v>
+        <v>-1.921612537705264E-2</v>
       </c>
       <c r="G48" s="11">
-        <v>-1.921612537705264E-2</v>
+        <v>-3.0237122579251263E-2</v>
       </c>
       <c r="H48" s="11">
-        <v>-3.0237122579251263E-2</v>
-      </c>
-      <c r="I48" s="11">
         <v>-3.135372788063262E-2</v>
       </c>
-      <c r="J48" s="12">
+      <c r="I48" s="12">
         <v>-3.3851917325144809E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="7">
         <v>2057</v>
       </c>
@@ -2094,22 +1947,19 @@
         <v>-1.4428817919254877E-2</v>
       </c>
       <c r="F49" s="8">
-        <v>-1.7862530884360295E-2</v>
+        <v>-1.970721584785573E-2</v>
       </c>
       <c r="G49" s="8">
-        <v>-1.970721584785573E-2</v>
+        <v>-3.0989303112399225E-2</v>
       </c>
       <c r="H49" s="8">
-        <v>-3.0989303112399225E-2</v>
-      </c>
-      <c r="I49" s="8">
         <v>-3.2665062311714288E-2</v>
       </c>
-      <c r="J49" s="9">
+      <c r="I49" s="9">
         <v>-3.4948435818108692E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="10">
         <v>2058</v>
       </c>
@@ -2126,22 +1976,19 @@
         <v>-1.4778370237727434E-2</v>
       </c>
       <c r="F50" s="11">
-        <v>-1.8556612293929908E-2</v>
+        <v>-2.0191139084108745E-2</v>
       </c>
       <c r="G50" s="11">
-        <v>-2.0191139084108745E-2</v>
+        <v>-3.1678904404835673E-2</v>
       </c>
       <c r="H50" s="11">
-        <v>-3.1678904404835673E-2</v>
-      </c>
-      <c r="I50" s="11">
         <v>-3.4030654054330145E-2</v>
       </c>
-      <c r="J50" s="12">
+      <c r="I50" s="12">
         <v>-3.6080132868398618E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="7">
         <v>2059</v>
       </c>
@@ -2158,22 +2005,19 @@
         <v>-1.5090307849834561E-2</v>
       </c>
       <c r="F51" s="8">
-        <v>-1.927861559829025E-2</v>
+        <v>-2.0682450061808244E-2</v>
       </c>
       <c r="G51" s="8">
-        <v>-2.0682450061808244E-2</v>
+        <v>-3.2378670638648521E-2</v>
       </c>
       <c r="H51" s="8">
-        <v>-3.2378670638648521E-2</v>
-      </c>
-      <c r="I51" s="8">
         <v>-3.5462657758975946E-2</v>
       </c>
-      <c r="J51" s="9">
+      <c r="I51" s="9">
         <v>-3.7299919932123338E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="13">
         <v>2060</v>
       </c>
@@ -2190,24 +2034,21 @@
         <v>-1.5425201489287832E-2</v>
       </c>
       <c r="F52" s="14">
-        <v>-2.0019826963589504E-2</v>
+        <v>-2.117196255716014E-2</v>
       </c>
       <c r="G52" s="14">
-        <v>-2.117196255716014E-2</v>
+        <v>-3.3046851828455459E-2</v>
       </c>
       <c r="H52" s="14">
-        <v>-3.3046851828455459E-2</v>
-      </c>
-      <c r="I52" s="14">
         <v>-3.6963763664746629E-2</v>
       </c>
-      <c r="J52" s="15">
+      <c r="I52" s="15">
         <v>-3.8461210125570577E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B53" s="8">
         <v>-1.1715621926770003E-3</v>
@@ -2222,24 +2063,21 @@
         <v>-7.5421107283699662E-3</v>
       </c>
       <c r="F53" s="8">
-        <v>-9.5224587245733572E-3</v>
+        <v>-1.0307149416342587E-2</v>
       </c>
       <c r="G53" s="8">
-        <v>-1.0307149416342587E-2</v>
+        <v>-1.6233216946482831E-2</v>
       </c>
       <c r="H53" s="8">
-        <v>-1.6233216946482831E-2</v>
-      </c>
-      <c r="I53" s="8">
         <v>-1.6984456577627705E-2</v>
       </c>
-      <c r="J53" s="9">
+      <c r="I53" s="9">
         <v>-1.8743579580162373E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B54" s="14">
         <v>-2.5055205220351207E-3</v>
@@ -2254,31 +2092,28 @@
         <v>-1.6465683061547831E-2</v>
       </c>
       <c r="F54" s="14">
-        <v>-2.3622632067094695E-2</v>
+        <v>-2.2590352418530135E-2</v>
       </c>
       <c r="G54" s="14">
-        <v>-2.2590352418530135E-2</v>
+        <v>-3.4896581300609797E-2</v>
       </c>
       <c r="H54" s="14">
-        <v>-3.4896581300609797E-2</v>
-      </c>
-      <c r="I54" s="14">
         <v>-4.9271263248319208E-2</v>
       </c>
-      <c r="J54" s="15">
+      <c r="I54" s="15">
         <v>-4.1137128679647694E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>